<commit_message>
✅ Final updates: database seeded, QR generated, and full report exported
</commit_message>
<xml_diff>
--- a/exports/AI_full_report.xlsx
+++ b/exports/AI_full_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,11 @@
           <t>Name</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>2025-07-03</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -456,6 +461,11 @@
           <t>Anshika Bharti</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -468,6 +478,11 @@
           <t>Rohan Verma</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -480,6 +495,11 @@
           <t>Priya Kapoor</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -492,6 +512,11 @@
           <t>Drishti paras</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -502,6 +527,11 @@
       <c r="B6" t="inlineStr">
         <is>
           <t>Ishan sharma</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>A</t>
         </is>
       </c>
     </row>

</xml_diff>